<commit_message>
docs: update monday board export
</commit_message>
<xml_diff>
--- a/public/files/projects/masita/general/monday-board.xlsx
+++ b/public/files/projects/masita/general/monday-board.xlsx
@@ -17,7 +17,7 @@
     <numFmt numFmtId="103" formatCode="YYYY-MM-DD HH:mm"/>
     <numFmt numFmtId="104" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="49">
+  <fonts count="48">
     <font>
       <name val="Arial"/>
       <sz val="11"/>
@@ -312,9 +312,10 @@
     </font>
     <font>
       <name val="Arial"/>
-      <sz val="11"/>
+      <sz val="14"/>
       <family val="1"/>
-      <color rgb="FFFFFFFF"/>
+      <b val="1"/>
+      <color rgb="FFCAB641"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -322,15 +323,8 @@
       <family val="1"/>
       <color rgb="FFFFFFFF"/>
     </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="14"/>
-      <family val="1"/>
-      <b val="1"/>
-      <color rgb="FFCAB641"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,7 +473,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC4C4C4"/>
+        <fgColor rgb="FF9D50DD"/>
       </patternFill>
     </fill>
     <fill>
@@ -489,12 +483,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9D50DD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC4C4C4"/>
+        <fgColor rgb="FFFDAB3D"/>
       </patternFill>
     </fill>
     <fill>
@@ -504,11 +493,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF401694"/>
+        <fgColor rgb="FFC4C4C4"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="29">
     <border/>
     <border>
       <left style="thin">
@@ -834,16 +823,16 @@
     </border>
     <border>
       <left style="thick">
-        <color rgb="FFB0B0B0"/>
+        <color rgb="FF9238AF"/>
       </left>
       <right style="thick">
-        <color rgb="FFB0B0B0"/>
+        <color rgb="FF9238AF"/>
       </right>
       <top style="thick">
-        <color rgb="FFB0B0B0"/>
+        <color rgb="FF9238AF"/>
       </top>
       <bottom style="thick">
-        <color rgb="FFB0B0B0"/>
+        <color rgb="FF9238AF"/>
       </bottom>
     </border>
     <border>
@@ -862,30 +851,16 @@
     </border>
     <border>
       <left style="thick">
-        <color rgb="FF9238AF"/>
+        <color rgb="FFE99729"/>
       </left>
       <right style="thick">
-        <color rgb="FF9238AF"/>
+        <color rgb="FFE99729"/>
       </right>
       <top style="thick">
-        <color rgb="FF9238AF"/>
+        <color rgb="FFE99729"/>
       </top>
       <bottom style="thick">
-        <color rgb="FF9238AF"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFB0B0B0"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFB0B0B0"/>
-      </right>
-      <top style="thick">
-        <color rgb="FFB0B0B0"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFB0B0B0"/>
+        <color rgb="FFE99729"/>
       </bottom>
     </border>
     <border>
@@ -904,23 +879,23 @@
     </border>
     <border>
       <left style="thick">
-        <color rgb="FF401694"/>
+        <color rgb="FFB0B0B0"/>
       </left>
       <right style="thick">
-        <color rgb="FF401694"/>
+        <color rgb="FFB0B0B0"/>
       </right>
       <top style="thick">
-        <color rgb="FF401694"/>
+        <color rgb="FFB0B0B0"/>
       </top>
       <bottom style="thick">
-        <color rgb="FF401694"/>
+        <color rgb="FFB0B0B0"/>
       </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
@@ -1071,14 +1046,11 @@
     <xf borderId="27" numFmtId="0" fontId="45" fillId="33" applyNumberFormat="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="28" numFmtId="0" fontId="46" fillId="34" applyNumberFormat="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf borderId="0" numFmtId="0" fontId="46" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="28" numFmtId="0" fontId="47" fillId="34" applyNumberFormat="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="29" numFmtId="0" fontId="47" fillId="35" applyNumberFormat="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="0" numFmtId="0" fontId="48" fillId="0" applyNumberFormat="0" applyFill="0" applyFont="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1134,7 +1106,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F200"/>
+  <dimension ref="A1:F199"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -5867,17 +5839,17 @@
     <row customHeight="1" ht="20" r="166">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>Tests opzetten voor must-haves</t>
-        </is>
-      </c>
-      <c r="B166" s="48" t="inlineStr">
-        <is>
-          <t>Not started</t>
-        </is>
-      </c>
-      <c r="C166" s="20" t="inlineStr">
-        <is>
-          <t>S: 1 - 3 uur</t>
+          <t>Portfolio updaten (laatste keer)</t>
+        </is>
+      </c>
+      <c r="B166" s="23" t="inlineStr">
+        <is>
+          <t>On hold</t>
+        </is>
+      </c>
+      <c r="C166" s="25" t="inlineStr">
+        <is>
+          <t>XL: &gt; 16 uur</t>
         </is>
       </c>
       <c r="D166" s="18" t="inlineStr">
@@ -5890,69 +5862,71 @@
       </c>
       <c r="F166" s="14" t="inlineStr">
         <is>
-          <t/>
+          <t>All research documents same format, same font (inter), latest version uploaded as pdf, Updated reading guide both online and local (pdf), All posts have correct learning outcomes on both online and local reading guide, Reflectie leeruitkomst 5 maken en content toevoegen, Content development toevoegen, Archiveren portfolio, Leeruitkomst 1+5 midterm review content toevoegen, Monday board exporteren en toevoegen aan agile methodology, Reading guide hoofd/subvragen conclusies toevoegen, Feedback Luuk/Robin verwerken, Final prototype recording maken en op het einde toevoegen aan portfolio</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="20" r="167">
-      <c r="A167" s="3" t="inlineStr">
-        <is>
-          <t>Portfolio updaten (laatste keer)</t>
-        </is>
-      </c>
-      <c r="B167" s="49" t="inlineStr">
-        <is>
-          <t>Working on it</t>
-        </is>
-      </c>
-      <c r="C167" s="25" t="inlineStr">
-        <is>
-          <t>XL: &gt; 16 uur</t>
-        </is>
-      </c>
-      <c r="D167" s="18" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="E167" s="13">
-        <v>45457.0</v>
-      </c>
-      <c r="F167" s="14" t="inlineStr">
-        <is>
-          <t>All research documents same format, same font (inter), latest version uploaded as pdf, Updated reading guide both online and local (pdf), All posts have correct learning outcomes on both online and local reading guide, Reflectie leeruitkomst 5 maken en content toevoegen, Iets voor leeruitkomst 5/6 qua communicatie en rol in een team?, Content development toevoegen, Archiveren portfolio, Leeruitkomst 1+5 midterm review content toevoegen, Monday board exporteren en toevoegen aan agile methodology, Pdf links omzetten in interne pdf viewer met fancybox?</t>
+      <c r="A167" s="10" t="inlineStr">
+        <is>
+          <t>Subitems</t>
+        </is>
+      </c>
+      <c r="B167" s="9" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C167" s="8" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D167" s="8" t="inlineStr">
+        <is>
+          <t>Estimated hours</t>
+        </is>
+      </c>
+      <c r="E167" s="8" t="inlineStr">
+        <is>
+          <t>Priority</t>
+        </is>
+      </c>
+      <c r="F167" s="8" t="inlineStr">
+        <is>
+          <t>Priority</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="20" r="168">
-      <c r="A168" s="10" t="inlineStr">
-        <is>
-          <t>Subitems</t>
-        </is>
-      </c>
-      <c r="B168" s="9" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C168" s="8" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="D168" s="8" t="inlineStr">
-        <is>
-          <t>Estimated hours</t>
-        </is>
-      </c>
-      <c r="E168" s="8" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
-      <c r="F168" s="8" t="inlineStr">
-        <is>
-          <t>Priority</t>
+      <c r="A168" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B168" s="3" t="inlineStr">
+        <is>
+          <t>All research documents same format, same font (inter), latest version uploaded as pdf</t>
+        </is>
+      </c>
+      <c r="C168" s="29" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="D168" s="30" t="inlineStr">
+        <is>
+          <t>XS: &lt; 1 uur</t>
+        </is>
+      </c>
+      <c r="E168" s="14" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F168" s="31" t="inlineStr">
+        <is>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -5964,7 +5938,7 @@
       </c>
       <c r="B169" s="3" t="inlineStr">
         <is>
-          <t>All research documents same format, same font (inter), latest version uploaded as pdf</t>
+          <t>Reflectie leeruitkomst 5 maken en content toevoegen</t>
         </is>
       </c>
       <c r="C169" s="29" t="inlineStr">
@@ -5972,9 +5946,9 @@
           <t>Done</t>
         </is>
       </c>
-      <c r="D169" s="41" t="inlineStr">
-        <is>
-          <t>Needs estimation</t>
+      <c r="D169" s="34" t="inlineStr">
+        <is>
+          <t>S: 1 - 3 uur</t>
         </is>
       </c>
       <c r="E169" s="14" t="inlineStr">
@@ -5996,7 +5970,7 @@
       </c>
       <c r="B170" s="3" t="inlineStr">
         <is>
-          <t>Reflectie leeruitkomst 5 maken en content toevoegen</t>
+          <t>Updated reading guide both online and local (pdf)</t>
         </is>
       </c>
       <c r="C170" s="29" t="inlineStr">
@@ -6004,9 +5978,9 @@
           <t>Done</t>
         </is>
       </c>
-      <c r="D170" s="41" t="inlineStr">
-        <is>
-          <t>Needs estimation</t>
+      <c r="D170" s="30" t="inlineStr">
+        <is>
+          <t>XS: &lt; 1 uur</t>
         </is>
       </c>
       <c r="E170" s="14" t="inlineStr">
@@ -6028,7 +6002,7 @@
       </c>
       <c r="B171" s="3" t="inlineStr">
         <is>
-          <t>Updated reading guide both online and local (pdf)</t>
+          <t>All posts have correct learning outcomes on both online and local reading guide</t>
         </is>
       </c>
       <c r="C171" s="29" t="inlineStr">
@@ -6036,9 +6010,9 @@
           <t>Done</t>
         </is>
       </c>
-      <c r="D171" s="41" t="inlineStr">
-        <is>
-          <t>Needs estimation</t>
+      <c r="D171" s="30" t="inlineStr">
+        <is>
+          <t>XS: &lt; 1 uur</t>
         </is>
       </c>
       <c r="E171" s="14" t="inlineStr">
@@ -6060,17 +6034,17 @@
       </c>
       <c r="B172" s="3" t="inlineStr">
         <is>
-          <t>Iets voor leeruitkomst 5/6 qua communicatie en rol in een team?</t>
-        </is>
-      </c>
-      <c r="C172" s="50" t="inlineStr">
-        <is>
-          <t>On hold</t>
-        </is>
-      </c>
-      <c r="D172" s="41" t="inlineStr">
-        <is>
-          <t>Needs estimation</t>
+          <t>Content development toevoegen</t>
+        </is>
+      </c>
+      <c r="C172" s="29" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="D172" s="34" t="inlineStr">
+        <is>
+          <t>S: 1 - 3 uur</t>
         </is>
       </c>
       <c r="E172" s="14" t="inlineStr">
@@ -6092,7 +6066,7 @@
       </c>
       <c r="B173" s="3" t="inlineStr">
         <is>
-          <t>All posts have correct learning outcomes on both online and local reading guide</t>
+          <t>Leeruitkomst 1+5 midterm review content toevoegen</t>
         </is>
       </c>
       <c r="C173" s="29" t="inlineStr">
@@ -6100,9 +6074,9 @@
           <t>Done</t>
         </is>
       </c>
-      <c r="D173" s="41" t="inlineStr">
-        <is>
-          <t>Needs estimation</t>
+      <c r="D173" s="30" t="inlineStr">
+        <is>
+          <t>XS: &lt; 1 uur</t>
         </is>
       </c>
       <c r="E173" s="14" t="inlineStr">
@@ -6124,7 +6098,7 @@
       </c>
       <c r="B174" s="3" t="inlineStr">
         <is>
-          <t>Content development toevoegen</t>
+          <t>Monday board exporteren en toevoegen aan agile methodology</t>
         </is>
       </c>
       <c r="C174" s="29" t="inlineStr">
@@ -6132,9 +6106,9 @@
           <t>Done</t>
         </is>
       </c>
-      <c r="D174" s="41" t="inlineStr">
-        <is>
-          <t>Needs estimation</t>
+      <c r="D174" s="30" t="inlineStr">
+        <is>
+          <t>XS: &lt; 1 uur</t>
         </is>
       </c>
       <c r="E174" s="14" t="inlineStr">
@@ -6156,17 +6130,17 @@
       </c>
       <c r="B175" s="3" t="inlineStr">
         <is>
-          <t>Archiveren portfolio</t>
-        </is>
-      </c>
-      <c r="C175" s="51" t="inlineStr">
-        <is>
-          <t>Not started</t>
-        </is>
-      </c>
-      <c r="D175" s="41" t="inlineStr">
-        <is>
-          <t>Needs estimation</t>
+          <t>Reading guide hoofd/subvragen conclusies toevoegen</t>
+        </is>
+      </c>
+      <c r="C175" s="29" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="D175" s="30" t="inlineStr">
+        <is>
+          <t>XS: &lt; 1 uur</t>
         </is>
       </c>
       <c r="E175" s="14" t="inlineStr">
@@ -6188,17 +6162,17 @@
       </c>
       <c r="B176" s="3" t="inlineStr">
         <is>
-          <t>Leeruitkomst 1+5 midterm review content toevoegen</t>
-        </is>
-      </c>
-      <c r="C176" s="29" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="D176" s="41" t="inlineStr">
-        <is>
-          <t>Needs estimation</t>
+          <t>Archiveren portfolio</t>
+        </is>
+      </c>
+      <c r="C176" s="48" t="inlineStr">
+        <is>
+          <t>On hold</t>
+        </is>
+      </c>
+      <c r="D176" s="34" t="inlineStr">
+        <is>
+          <t>S: 1 - 3 uur</t>
         </is>
       </c>
       <c r="E176" s="14" t="inlineStr">
@@ -6220,17 +6194,17 @@
       </c>
       <c r="B177" s="3" t="inlineStr">
         <is>
-          <t>Monday board exporteren en toevoegen aan agile methodology</t>
-        </is>
-      </c>
-      <c r="C177" s="51" t="inlineStr">
-        <is>
-          <t>Not started</t>
-        </is>
-      </c>
-      <c r="D177" s="41" t="inlineStr">
-        <is>
-          <t>Needs estimation</t>
+          <t>Feedback Luuk/Robin verwerken</t>
+        </is>
+      </c>
+      <c r="C177" s="48" t="inlineStr">
+        <is>
+          <t>On hold</t>
+        </is>
+      </c>
+      <c r="D177" s="34" t="inlineStr">
+        <is>
+          <t>S: 1 - 3 uur</t>
         </is>
       </c>
       <c r="E177" s="14" t="inlineStr">
@@ -6252,17 +6226,17 @@
       </c>
       <c r="B178" s="3" t="inlineStr">
         <is>
-          <t>Pdf links omzetten in interne pdf viewer met fancybox?</t>
-        </is>
-      </c>
-      <c r="C178" s="50" t="inlineStr">
-        <is>
-          <t>On hold</t>
-        </is>
-      </c>
-      <c r="D178" s="41" t="inlineStr">
-        <is>
-          <t>Needs estimation</t>
+          <t>Final prototype recording maken en op het einde toevoegen aan portfolio</t>
+        </is>
+      </c>
+      <c r="C178" s="49" t="inlineStr">
+        <is>
+          <t>Working on it</t>
+        </is>
+      </c>
+      <c r="D178" s="30" t="inlineStr">
+        <is>
+          <t>XS: &lt; 1 uur</t>
         </is>
       </c>
       <c r="E178" s="14" t="inlineStr">
@@ -6282,14 +6256,14 @@
           <t>Backlog functies afwerken op basis van MoSCoW prioriteit</t>
         </is>
       </c>
-      <c r="B179" s="48" t="inlineStr">
-        <is>
-          <t>Not started</t>
-        </is>
-      </c>
-      <c r="C179" s="37" t="inlineStr">
-        <is>
-          <t>Needs estimation</t>
+      <c r="B179" s="50" t="inlineStr">
+        <is>
+          <t>Working on it</t>
+        </is>
+      </c>
+      <c r="C179" s="19" t="inlineStr">
+        <is>
+          <t>L: 8 - 16 uur</t>
         </is>
       </c>
       <c r="D179" s="18" t="inlineStr">
@@ -6302,7 +6276,7 @@
       </c>
       <c r="F179" s="14" t="inlineStr">
         <is>
-          <t>As a Masita employee, I want to be able to make basic changes to the content of my website, As a user, I want to be able to filter through a collection of products</t>
+          <t>As a Masita employee, I want to be able to make basic changes to the content of my website, As a user, I want to be able to filter through a collection of products, As a user, I want to be able to scroll through the content of my website on all devices (side-scroll)</t>
         </is>
       </c>
     </row>
@@ -6349,7 +6323,7 @@
           <t>As a Masita employee, I want to be able to make basic changes to the content of my website</t>
         </is>
       </c>
-      <c r="C181" s="50" t="inlineStr">
+      <c r="C181" s="48" t="inlineStr">
         <is>
           <t>On hold</t>
         </is>
@@ -6381,14 +6355,14 @@
           <t>As a user, I want to be able to filter through a collection of products</t>
         </is>
       </c>
-      <c r="C182" s="51" t="inlineStr">
-        <is>
-          <t>Not started</t>
-        </is>
-      </c>
-      <c r="D182" s="41" t="inlineStr">
-        <is>
-          <t>Needs estimation</t>
+      <c r="C182" s="49" t="inlineStr">
+        <is>
+          <t>Working on it</t>
+        </is>
+      </c>
+      <c r="D182" s="33" t="inlineStr">
+        <is>
+          <t>M: 3 - 8 uur</t>
         </is>
       </c>
       <c r="E182" s="14" t="inlineStr">
@@ -6405,94 +6379,94 @@
     <row customHeight="1" ht="20" r="183">
       <c r="A183" s="3" t="inlineStr">
         <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B183" s="3" t="inlineStr">
+        <is>
+          <t>As a user, I want to be able to scroll through the content of my website on all devices (side-scroll)</t>
+        </is>
+      </c>
+      <c r="C183" s="29" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="D183" s="30" t="inlineStr">
+        <is>
+          <t>XS: &lt; 1 uur</t>
+        </is>
+      </c>
+      <c r="E183" s="14" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F183" s="31" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="20" r="184">
+      <c r="A184" s="3" t="inlineStr">
+        <is>
           <t>Development could-haves</t>
         </is>
       </c>
-      <c r="B183" s="48" t="inlineStr">
-        <is>
-          <t>Not started</t>
-        </is>
-      </c>
-      <c r="C183" s="19" t="inlineStr">
+      <c r="B184" s="16" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="C184" s="19" t="inlineStr">
         <is>
           <t>L: 8 - 16 uur</t>
         </is>
       </c>
-      <c r="D183" s="18" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="E183" s="13">
+      <c r="D184" s="18" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E184" s="13">
         <v>45457.0</v>
       </c>
-      <c r="F183" s="14" t="inlineStr">
+      <c r="F184" s="14" t="inlineStr">
         <is>
           <t>As a developer, I want to be able to work with dynamic and scalable code, As a developer, I want to be able to re-use code snippets or elements for future e-commerce projects outside of this project, As a developer, I want to be able to set up and run proper unit / code tests, As a user, I want to be able to see product reviews</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="20" r="184">
-      <c r="A184" s="10" t="inlineStr">
+    <row customHeight="1" ht="20" r="185">
+      <c r="A185" s="10" t="inlineStr">
         <is>
           <t>Subitems</t>
         </is>
       </c>
-      <c r="B184" s="9" t="inlineStr">
+      <c r="B185" s="9" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C184" s="8" t="inlineStr">
+      <c r="C185" s="8" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="D184" s="8" t="inlineStr">
+      <c r="D185" s="8" t="inlineStr">
         <is>
           <t>Estimated hours</t>
         </is>
       </c>
-      <c r="E184" s="8" t="inlineStr">
+      <c r="E185" s="8" t="inlineStr">
         <is>
           <t>Priority</t>
         </is>
       </c>
-      <c r="F184" s="8" t="inlineStr">
+      <c r="F185" s="8" t="inlineStr">
         <is>
           <t>Priority</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="20" r="185">
-      <c r="A185" s="3" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="B185" s="3" t="inlineStr">
-        <is>
-          <t>As a user, I want to be able to see product reviews</t>
-        </is>
-      </c>
-      <c r="C185" s="51" t="inlineStr">
-        <is>
-          <t>Not started</t>
-        </is>
-      </c>
-      <c r="D185" s="41" t="inlineStr">
-        <is>
-          <t>Needs estimation</t>
-        </is>
-      </c>
-      <c r="E185" s="14" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F185" s="31" t="inlineStr">
-        <is>
-          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -6504,12 +6478,12 @@
       </c>
       <c r="B186" s="3" t="inlineStr">
         <is>
-          <t>As a developer, I want to be able to work with dynamic and scalable code</t>
-        </is>
-      </c>
-      <c r="C186" s="51" t="inlineStr">
-        <is>
-          <t>Not started</t>
+          <t>As a user, I want to be able to see product reviews</t>
+        </is>
+      </c>
+      <c r="C186" s="45" t="inlineStr">
+        <is>
+          <t>Out of scope</t>
         </is>
       </c>
       <c r="D186" s="41" t="inlineStr">
@@ -6522,9 +6496,9 @@
           <t/>
         </is>
       </c>
-      <c r="F186" s="52" t="inlineStr">
-        <is>
-          <t>Could have</t>
+      <c r="F186" s="31" t="inlineStr">
+        <is>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -6536,12 +6510,12 @@
       </c>
       <c r="B187" s="3" t="inlineStr">
         <is>
-          <t>As a developer, I want to be able to re-use code snippets or elements for future e-commerce projects outside of this project</t>
-        </is>
-      </c>
-      <c r="C187" s="51" t="inlineStr">
-        <is>
-          <t>Not started</t>
+          <t>As a developer, I want to be able to work with dynamic and scalable code</t>
+        </is>
+      </c>
+      <c r="C187" s="29" t="inlineStr">
+        <is>
+          <t>Done</t>
         </is>
       </c>
       <c r="D187" s="41" t="inlineStr">
@@ -6554,7 +6528,7 @@
           <t/>
         </is>
       </c>
-      <c r="F187" s="52" t="inlineStr">
+      <c r="F187" s="51" t="inlineStr">
         <is>
           <t>Could have</t>
         </is>
@@ -6568,12 +6542,12 @@
       </c>
       <c r="B188" s="3" t="inlineStr">
         <is>
-          <t>As a developer, I want to be able to set up and run proper unit / code tests</t>
-        </is>
-      </c>
-      <c r="C188" s="45" t="inlineStr">
-        <is>
-          <t>Out of scope</t>
+          <t>As a developer, I want to be able to re-use code snippets or elements for future e-commerce projects outside of this project</t>
+        </is>
+      </c>
+      <c r="C188" s="29" t="inlineStr">
+        <is>
+          <t>Done</t>
         </is>
       </c>
       <c r="D188" s="41" t="inlineStr">
@@ -6586,7 +6560,7 @@
           <t/>
         </is>
       </c>
-      <c r="F188" s="52" t="inlineStr">
+      <c r="F188" s="51" t="inlineStr">
         <is>
           <t>Could have</t>
         </is>
@@ -6595,47 +6569,49 @@
     <row customHeight="1" ht="20" r="189">
       <c r="A189" s="3" t="inlineStr">
         <is>
-          <t>Retrospective &amp; sprint demo voorbereiden/houden</t>
-        </is>
-      </c>
-      <c r="B189" s="53" t="inlineStr">
-        <is>
-          <t>On hold until sprint end</t>
-        </is>
-      </c>
-      <c r="C189" s="17" t="inlineStr">
-        <is>
-          <t>XS: &lt; 1 uur</t>
-        </is>
-      </c>
-      <c r="D189" s="18" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="E189" s="13">
-        <v>45457.0</v>
-      </c>
-      <c r="F189" s="14" t="inlineStr">
-        <is>
-          <t/>
+          <t/>
+        </is>
+      </c>
+      <c r="B189" s="3" t="inlineStr">
+        <is>
+          <t>As a developer, I want to be able to set up and run proper unit / code tests</t>
+        </is>
+      </c>
+      <c r="C189" s="45" t="inlineStr">
+        <is>
+          <t>Out of scope</t>
+        </is>
+      </c>
+      <c r="D189" s="41" t="inlineStr">
+        <is>
+          <t>Needs estimation</t>
+        </is>
+      </c>
+      <c r="E189" s="14" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F189" s="51" t="inlineStr">
+        <is>
+          <t>Could have</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="20" r="190">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>Tests uitvoeren voor must-haves</t>
-        </is>
-      </c>
-      <c r="B190" s="48" t="inlineStr">
-        <is>
-          <t>Not started</t>
-        </is>
-      </c>
-      <c r="C190" s="20" t="inlineStr">
-        <is>
-          <t>S: 1 - 3 uur</t>
+          <t>Retrospective &amp; sprint demo voorbereiden/houden</t>
+        </is>
+      </c>
+      <c r="B190" s="24" t="inlineStr">
+        <is>
+          <t>Unfinished</t>
+        </is>
+      </c>
+      <c r="C190" s="17" t="inlineStr">
+        <is>
+          <t>XS: &lt; 1 uur</t>
         </is>
       </c>
       <c r="D190" s="18" t="inlineStr">
@@ -6685,17 +6661,17 @@
     <row customHeight="1" ht="20" r="192">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>Final prototype recording maken en op het einde toevoegen aan portfolio</t>
-        </is>
-      </c>
-      <c r="B192" s="48" t="inlineStr">
-        <is>
-          <t>Not started</t>
-        </is>
-      </c>
-      <c r="C192" s="37" t="inlineStr">
-        <is>
-          <t>Needs estimation</t>
+          <t>Adviesrapport maken</t>
+        </is>
+      </c>
+      <c r="B192" s="16" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="C192" s="20" t="inlineStr">
+        <is>
+          <t>S: 1 - 3 uur</t>
         </is>
       </c>
       <c r="D192" s="18" t="inlineStr">
@@ -6748,7 +6724,7 @@
     </row>
     <row customHeight="1" ht="40" r="194"/>
     <row customHeight="1" ht="20" r="195">
-      <c r="A195" s="54" t="inlineStr">
+      <c r="A195" s="52" t="inlineStr">
         <is>
           <t>Sprint 8 - week 18 + 19 (week 25 &amp; 26 - 17 juni t/m 28 juni)</t>
         </is>
@@ -6792,7 +6768,7 @@
           <t>Overdracht documenten en andere benodigdheden</t>
         </is>
       </c>
-      <c r="B197" s="48" t="inlineStr">
+      <c r="B197" s="53" t="inlineStr">
         <is>
           <t>Not started</t>
         </is>
@@ -6819,10 +6795,10 @@
     <row customHeight="1" ht="20" r="198">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>Adviesrapport maken?</t>
-        </is>
-      </c>
-      <c r="B198" s="48" t="inlineStr">
+          <t>Voorbereiden presentatie</t>
+        </is>
+      </c>
+      <c r="B198" s="53" t="inlineStr">
         <is>
           <t>Not started</t>
         </is>
@@ -6847,62 +6823,32 @@
       </c>
     </row>
     <row customHeight="1" ht="20" r="199">
-      <c r="A199" s="3" t="inlineStr">
-        <is>
-          <t>Voorbereiden presentatie</t>
-        </is>
-      </c>
-      <c r="B199" s="48" t="inlineStr">
-        <is>
-          <t>Not started</t>
-        </is>
-      </c>
-      <c r="C199" s="22" t="inlineStr">
-        <is>
-          <t>M: 3 - 8 uur</t>
-        </is>
-      </c>
-      <c r="D199" s="18" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="E199" s="13">
-        <v>45471.0</v>
-      </c>
-      <c r="F199" s="14" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="20" r="200">
-      <c r="A200" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="B200" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C200" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D200" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E200" s="26" t="inlineStr">
+      <c r="A199" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B199" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C199" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D199" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E199" s="26" t="inlineStr">
         <is>
           <t>2024-06-28</t>
         </is>
       </c>
-      <c r="F200" s="0" t="inlineStr">
+      <c r="F199" s="0" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>